<commit_message>
change similarity to phash and resources image&pdf merge files floder
</commit_message>
<xml_diff>
--- a/pc_scand/resources/case.xlsx
+++ b/pc_scand/resources/case.xlsx
@@ -1,196 +1,231 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="13810" windowHeight="6860" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView windowWidth="18530" windowHeight="7010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Case" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="JiyinScan" sheetId="1" r:id="rId1"/>
+    <sheet name="PanelScan" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="144525" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+  <si>
+    <t>结果</t>
+  </si>
+  <si>
+    <t>备注</t>
+  </si>
+  <si>
+    <t>连接方式</t>
+  </si>
+  <si>
+    <t>纸张来源</t>
+  </si>
+  <si>
+    <t>色彩模式</t>
+  </si>
+  <si>
+    <t>纸张大小</t>
+  </si>
+  <si>
+    <t>分辨率</t>
+  </si>
+  <si>
+    <t>保存格式</t>
+  </si>
+  <si>
+    <t>Scaling_ratio</t>
+  </si>
+  <si>
+    <t>单双面</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="23">
-    <font>
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <color theme="1"/>
-      <sz val="12"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8"/>
+      <color rgb="FF067D17"/>
       <name val="Courier New"/>
       <charset val="134"/>
-      <color rgb="FF067D17"/>
-      <sz val="9.800000000000001"/>
-    </font>
-    <font>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF3F3F76"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF9C0006"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color theme="0"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF0000FF"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF800080"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FFFF0000"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="18"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="15"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="13"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FF3F3F3F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <color theme="1"/>
-      <sz val="12"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -491,157 +526,154 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyAlignment="1">
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -697,74 +729,11 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1088,82 +1057,116 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:H13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col width="12.8" customWidth="1" min="1" max="1"/>
-    <col width="45.9166666666667" customWidth="1" min="2" max="2"/>
-    <col width="15.8416666666667" customWidth="1" min="3" max="3"/>
-    <col width="16.9583333333333" customWidth="1" min="4" max="4"/>
-    <col width="16.8" customWidth="1" min="5" max="5"/>
-    <col width="16.3166666666667" customWidth="1" min="6" max="6"/>
-    <col width="12.8" customWidth="1" min="7" max="7"/>
-    <col width="15.5166666666667" customWidth="1" min="8" max="8"/>
-    <col width="15.3583333333333" customWidth="1" min="9" max="9"/>
-    <col width="17.6" customWidth="1" min="10" max="10"/>
-    <col width="13.6" customWidth="1" min="11" max="11"/>
-    <col width="18.5583333333333" customWidth="1" min="12" max="12"/>
-    <col width="20" customWidth="1" min="13" max="13"/>
+    <col min="1" max="1" width="12.8" customWidth="1"/>
+    <col min="2" max="2" width="45.9166666666667" customWidth="1"/>
+    <col min="3" max="3" width="15.8416666666667" customWidth="1"/>
+    <col min="4" max="4" width="16.9583333333333" customWidth="1"/>
+    <col min="5" max="5" width="16.8" customWidth="1"/>
+    <col min="6" max="6" width="16.3166666666667" customWidth="1"/>
+    <col min="7" max="7" width="12.8" customWidth="1"/>
+    <col min="8" max="8" width="15.5166666666667" customWidth="1"/>
+    <col min="9" max="9" width="15.3583333333333" customWidth="1"/>
+    <col min="10" max="10" width="17.6" customWidth="1"/>
+    <col min="11" max="11" width="13.6" customWidth="1"/>
+    <col min="12" max="12" width="18.5583333333333" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26" customHeight="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>结果</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>备注</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>连接方式</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>纸张来源</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>色彩模式</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>纸张大小</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>分辨率</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>保存格式</t>
-        </is>
-      </c>
-      <c r="N1" s="2" t="inlineStr">
-        <is>
-          <t>Scaling_ratio</t>
-        </is>
+    <row r="1" ht="26" customHeight="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="29.9166666666667" customWidth="1"/>
+    <col min="3" max="3" width="20.1666666666667" customWidth="1"/>
+    <col min="4" max="4" width="13.6666666666667" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="12.9166666666667" customWidth="1"/>
+    <col min="7" max="7" width="16.8333333333333" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="26" customHeight="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>